<commit_message>
Commit of Incentive plan exel and pdf, Manufacturing Plant exel and pdf, and the Sales org pdf
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Sales_Org.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Sales_Org.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjpry\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C2A629-02F0-49A1-938B-66501224D999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6CE10D-44FE-458D-A7A9-8613FA4E163F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -291,6 +291,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,15 +307,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -625,7 +625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -715,11 +715,11 @@
       <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
@@ -809,11 +809,11 @@
       <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>

</xml_diff>

<commit_message>
Alteration of Mapping_Sales_Org, and addition of SSDT drawings
</commit_message>
<xml_diff>
--- a/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Sales_Org.xlsx
+++ b/Team_02_M2_Final_Submission/Team_02_M2_D1_Dimension_Mapping_metadata/support/Team_02_M2_D1_Dimension_Mapping_Sales_Org.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjpry\Desktop\M2\work\Team_02_M2_Final_Submission\Team_02_M2_D1_Dimension_Mapping_metadata\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6CE10D-44FE-458D-A7A9-8613FA4E163F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8ADC7C-AECA-4DDE-918E-AAD34FC9CD3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="35">
   <si>
     <t>Database</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Source-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -241,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -309,6 +312,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -735,10 +739,10 @@
         <v>23</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
@@ -761,10 +765,10 @@
         <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -787,7 +791,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>25</v>
@@ -835,10 +839,10 @@
         <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -861,10 +865,10 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -887,7 +891,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>25</v>
@@ -1035,6 +1039,11 @@
       </c>
       <c r="L15" s="8" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="33" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>